<commit_message>
Implemented email and username normalization in UsersCollect method
</commit_message>
<xml_diff>
--- a/Cinema.Test/TestDatabase/TestCinemaDatabase.xlsx
+++ b/Cinema.Test/TestDatabase/TestCinemaDatabase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Cinema\Cinema.Test\TestDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370658B6-58EF-4374-BE18-99C545008574}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754A2332-5722-4FB1-A8B0-2590CA07DF45}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="825" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="825" firstSheet="7" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pricings" sheetId="12" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="Users" sheetId="18" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Reservations'!$B$1:$F$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Reservations!$B$1:$F$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Seat!$A$1:$C$481</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">SeatReservations!$A$1:$E$62</definedName>
   </definedNames>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="280">
   <si>
     <t>Id</t>
   </si>
@@ -796,90 +796,60 @@
     <t>AppRole</t>
   </si>
   <si>
-    <t>979ed5506bb4fdb1db9378e5d757636cdb3a433e017fcab57b0ac2aa0a17f064</t>
-  </si>
-  <si>
     <t>Camille</t>
   </si>
   <si>
     <t>Coning</t>
   </si>
   <si>
-    <t>374a3179b04721bb813f37541e1a9d11ba8ea7760e3d43dd338248944487b7a5</t>
-  </si>
-  <si>
     <t>Mattie</t>
   </si>
   <si>
     <t>Alonso</t>
   </si>
   <si>
-    <t>be6c5cd9c3ce1fe60c794302d54168f220b1a7d375005abe71ef2e5a89b0cd9b</t>
-  </si>
-  <si>
     <t>Marylin</t>
   </si>
   <si>
     <t>Digweed</t>
   </si>
   <si>
-    <t>bd53763efe340395e8ab0059e8c2e43ca015a70a6a4cbc0fa5df084861f3b02a</t>
-  </si>
-  <si>
     <t>Gerri</t>
   </si>
   <si>
     <t>Beagles</t>
   </si>
   <si>
-    <t>05d186cc78d1e3179ff018d4f07ac39e8f85a97941f1bc33c96125ecf4ffc4c7</t>
-  </si>
-  <si>
     <t>Frannie</t>
   </si>
   <si>
     <t>Yoskowitz</t>
   </si>
   <si>
-    <t>7eebc1470934a6cb35182a6e991874829a6b39d06655005b014382b874f4acb6</t>
-  </si>
-  <si>
     <t>Geoff</t>
   </si>
   <si>
     <t>Scyone</t>
   </si>
   <si>
-    <t>4f1eb5be03772bbfcc12ee97b29cae3ee2b49a43eceb8d87b3dd549b3cf9125b</t>
-  </si>
-  <si>
     <t>Willie</t>
   </si>
   <si>
     <t>Baxill</t>
   </si>
   <si>
-    <t>4368e0e38bac123655c727af74a7dcee3b35b8be259866ad96270539946a9f99</t>
-  </si>
-  <si>
     <t>Laughton</t>
   </si>
   <si>
     <t>Skeldinge</t>
   </si>
   <si>
-    <t>b5442facd7e81dbdd0ae199aad2ae3f371d2b95d1c4c3b0495f49df4232debe3</t>
-  </si>
-  <si>
     <t>Emile</t>
   </si>
   <si>
     <t>Theunissen</t>
   </si>
   <si>
-    <t>18b8eab87f2558499795d23dba9e78606efa7cd7301c61b5ab9c82a40047aa3a</t>
-  </si>
-  <si>
     <t>Jock</t>
   </si>
   <si>
@@ -920,6 +890,9 @@
   </si>
   <si>
     <t>OrderNumber</t>
+  </si>
+  <si>
+    <t>P4$$W0RD123#</t>
   </si>
 </sst>
 </file>
@@ -1319,7 +1292,7 @@
       <calculatedColumnFormula>INDEX(Screenings[Hall],MATCH(Reservations[[#This Row],[Test_Screening]],Screenings[Test_Id],0))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{02492577-30BC-4736-89A6-7BCB43316500}" name="Number of SeatReservations" dataDxfId="12" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>COUNTIF(SeatReservations!G:G,'Reservations'!G2)</calculatedColumnFormula>
+      <calculatedColumnFormula>COUNTIF(SeatReservations!G:G,Reservations!G2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{6629A0B4-1EED-4F00-8980-01C1615D1E46}" name="Movie" dataDxfId="11" dataCellStyle="Normal 2">
       <calculatedColumnFormula>INDEX(Screenings[Movie],MATCH(Reservations[[#This Row],[Test_Screening]],Screenings[Test_Id],0))</calculatedColumnFormula>
@@ -3128,13 +3101,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>154</v>
@@ -3170,7 +3143,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G2)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G2)</f>
         <v>0</v>
       </c>
       <c r="F2" s="4">
@@ -3202,7 +3175,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G3)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G3)</f>
         <v>0</v>
       </c>
       <c r="F3" s="4">
@@ -3234,7 +3207,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G4)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G4)</f>
         <v>0</v>
       </c>
       <c r="F4" s="4">
@@ -3266,7 +3239,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G5)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G5)</f>
         <v>0</v>
       </c>
       <c r="F5" s="4">
@@ -3298,7 +3271,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G6)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G6)</f>
         <v>0</v>
       </c>
       <c r="F6" s="4">
@@ -3330,7 +3303,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G7)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G7)</f>
         <v>0</v>
       </c>
       <c r="F7" s="4">
@@ -3362,7 +3335,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G8)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G8)</f>
         <v>0</v>
       </c>
       <c r="F8" s="4">
@@ -3394,7 +3367,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G9)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G9)</f>
         <v>0</v>
       </c>
       <c r="F9" s="4">
@@ -3426,7 +3399,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G10)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G10)</f>
         <v>0</v>
       </c>
       <c r="F10" s="4">
@@ -3458,7 +3431,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G11)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G11)</f>
         <v>0</v>
       </c>
       <c r="F11" s="4">
@@ -3490,7 +3463,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G12)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G12)</f>
         <v>0</v>
       </c>
       <c r="F12" s="4">
@@ -3522,7 +3495,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G13)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G13)</f>
         <v>0</v>
       </c>
       <c r="F13" s="4">
@@ -3554,7 +3527,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G14)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G14)</f>
         <v>0</v>
       </c>
       <c r="F14" s="4">
@@ -3586,7 +3559,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G15)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G15)</f>
         <v>0</v>
       </c>
       <c r="F15" s="4">
@@ -3618,7 +3591,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G16)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G16)</f>
         <v>0</v>
       </c>
       <c r="F16" s="4">
@@ -3650,7 +3623,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G17)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G17)</f>
         <v>0</v>
       </c>
       <c r="F17" s="4">
@@ -3682,7 +3655,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G18)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G18)</f>
         <v>0</v>
       </c>
       <c r="F18" s="4">
@@ -3714,7 +3687,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G19)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G19)</f>
         <v>0</v>
       </c>
       <c r="F19" s="4">
@@ -3746,7 +3719,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G20)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G20)</f>
         <v>0</v>
       </c>
       <c r="F20" s="4">
@@ -3778,7 +3751,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G21)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G21)</f>
         <v>0</v>
       </c>
       <c r="F21" s="4">
@@ -3810,7 +3783,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G22)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G22)</f>
         <v>0</v>
       </c>
       <c r="F22" s="4">
@@ -3842,7 +3815,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G23)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G23)</f>
         <v>0</v>
       </c>
       <c r="F23" s="4">
@@ -3874,7 +3847,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G24)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G24)</f>
         <v>0</v>
       </c>
       <c r="F24" s="4">
@@ -3906,7 +3879,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G25)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G25)</f>
         <v>0</v>
       </c>
       <c r="F25" s="4">
@@ -3938,7 +3911,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G26)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G26)</f>
         <v>0</v>
       </c>
       <c r="F26" s="4">
@@ -3970,7 +3943,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="4">
-        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G27)</f>
+        <f>COUNTIF(SeatReservations!G:G,Reservations!G27)</f>
         <v>0</v>
       </c>
       <c r="F27" s="4">
@@ -4022,7 +3995,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>199</v>
@@ -4034,7 +4007,7 @@
         <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>9</v>
@@ -4059,7 +4032,7 @@
       </c>
       <c r="E2" s="6">
         <f t="shared" ref="E2" ca="1" si="0">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.91666666666666663</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="F2" s="15">
         <v>43513.618055555555</v>
@@ -4084,7 +4057,7 @@
       </c>
       <c r="E3" s="6">
         <f t="shared" ref="E3:E6" ca="1" si="1">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.78472222222222221</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="F3" s="15">
         <v>43680.631944444445</v>
@@ -4109,7 +4082,7 @@
       </c>
       <c r="E4" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.95138888888888884</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="F4" s="15">
         <v>43698.944444444445</v>
@@ -4134,7 +4107,7 @@
       </c>
       <c r="E5" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86111111111111116</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="F5" s="15">
         <v>43674.729166666664</v>
@@ -4159,7 +4132,7 @@
       </c>
       <c r="E6" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.54166666666666663</v>
+        <v>0.80555555555555547</v>
       </c>
       <c r="F6" s="15">
         <v>43730.590277777781</v>
@@ -4184,7 +4157,7 @@
       </c>
       <c r="E7" s="6">
         <f t="shared" ref="E7:E8" ca="1" si="2">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.82638888888888884</v>
+        <v>0.56944444444444442</v>
       </c>
       <c r="F7" s="15">
         <v>43430.916666666664</v>
@@ -4209,7 +4182,7 @@
       </c>
       <c r="E8" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>0.84722222222222221</v>
+        <v>0.71527777777777779</v>
       </c>
       <c r="F8" s="15">
         <v>43674.826388888891</v>
@@ -4234,7 +4207,7 @@
       </c>
       <c r="E9" s="6">
         <f t="shared" ref="E9" ca="1" si="3">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.58333333333333337</v>
+        <v>0.875</v>
       </c>
       <c r="F9" s="15">
         <v>43459.861111111109</v>
@@ -4284,7 +4257,7 @@
       </c>
       <c r="E11" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.79861111111111116</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="F11" s="15">
         <v>43552.6875</v>
@@ -4309,7 +4282,7 @@
       </c>
       <c r="E12" s="6">
         <f t="shared" ref="E12:E18" ca="1" si="5">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.79166666666666663</v>
+        <v>0.95138888888888884</v>
       </c>
       <c r="F12" s="15">
         <v>43430.611111111109</v>
@@ -4334,7 +4307,7 @@
       </c>
       <c r="E13" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.75</v>
+        <v>0.80555555555555547</v>
       </c>
       <c r="F13" s="15">
         <v>43737.923611111109</v>
@@ -4359,7 +4332,7 @@
       </c>
       <c r="E14" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.68055555555555547</v>
+        <v>0.70138888888888884</v>
       </c>
       <c r="F14" s="15">
         <v>43705.868055555555</v>
@@ -4384,7 +4357,7 @@
       </c>
       <c r="E15" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.59722222222222221</v>
+        <v>0.94444444444444453</v>
       </c>
       <c r="F15" s="15">
         <v>43738.881944444445</v>
@@ -4409,7 +4382,7 @@
       </c>
       <c r="E16" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.77083333333333337</v>
+        <v>0.56944444444444442</v>
       </c>
       <c r="F16" s="15">
         <v>43434.569444444445</v>
@@ -4434,7 +4407,7 @@
       </c>
       <c r="E17" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.86111111111111116</v>
+        <v>0.8125</v>
       </c>
       <c r="F17" s="15">
         <v>43613.944444444445</v>
@@ -4459,7 +4432,7 @@
       </c>
       <c r="E18" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.9375</v>
+        <v>0.90972222222222221</v>
       </c>
       <c r="F18" s="15">
         <v>43666.847222222219</v>
@@ -4484,7 +4457,7 @@
       </c>
       <c r="E19" s="6">
         <f t="shared" ref="E19:E23" ca="1" si="6">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.89583333333333337</v>
+        <v>0.95138888888888884</v>
       </c>
       <c r="F19" s="15">
         <v>43694.951388888891</v>
@@ -4509,7 +4482,7 @@
       </c>
       <c r="E20" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.67361111111111116</v>
+        <v>0.8125</v>
       </c>
       <c r="F20" s="15">
         <v>43661.854166666664</v>
@@ -4534,7 +4507,7 @@
       </c>
       <c r="E21" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.66666666666666663</v>
+        <v>0.57638888888888895</v>
       </c>
       <c r="F21" s="15">
         <v>43629.652777777781</v>
@@ -4559,7 +4532,7 @@
       </c>
       <c r="E22" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.57638888888888895</v>
+        <v>0.84722222222222221</v>
       </c>
       <c r="F22" s="15">
         <v>43430.847222222219</v>
@@ -4584,7 +4557,7 @@
       </c>
       <c r="E23" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.75</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="F23" s="15">
         <v>43632.618055555555</v>
@@ -4609,7 +4582,7 @@
       </c>
       <c r="E24" s="6">
         <f t="shared" ref="E24:E29" ca="1" si="7">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.86111111111111116</v>
+        <v>0.90972222222222221</v>
       </c>
       <c r="F24" s="15">
         <v>43731.548611111109</v>
@@ -4634,7 +4607,7 @@
       </c>
       <c r="E25" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.85416666666666663</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="F25" s="15">
         <v>43769.847222222219</v>
@@ -4659,7 +4632,7 @@
       </c>
       <c r="E26" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.79166666666666663</v>
+        <v>0.86111111111111116</v>
       </c>
       <c r="F26" s="15">
         <v>43508.583333333336</v>
@@ -4684,7 +4657,7 @@
       </c>
       <c r="E27" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.75</v>
+        <v>0.78472222222222221</v>
       </c>
       <c r="F27" s="15">
         <v>43441.548611111109</v>
@@ -4709,7 +4682,7 @@
       </c>
       <c r="E28" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.63888888888888895</v>
+        <v>0.84722222222222221</v>
       </c>
       <c r="F28" s="15">
         <v>43725.75</v>
@@ -4734,7 +4707,7 @@
       </c>
       <c r="E29" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.75</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="F29" s="15">
         <v>43639.694444444445</v>
@@ -4759,7 +4732,7 @@
       </c>
       <c r="E30" s="6">
         <f t="shared" ref="E30" ca="1" si="8">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.72222222222222221</v>
+        <v>0.75</v>
       </c>
       <c r="F30" s="15">
         <v>43704.902777777781</v>
@@ -4784,7 +4757,7 @@
       </c>
       <c r="E31" s="6">
         <f t="shared" ref="E31:E36" ca="1" si="9">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.72916666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="F31" s="15">
         <v>43727.638888888891</v>
@@ -4809,7 +4782,7 @@
       </c>
       <c r="E32" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>0.84722222222222221</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="F32" s="15">
         <v>43773.715277777781</v>
@@ -4834,7 +4807,7 @@
       </c>
       <c r="E33" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>0.61805555555555558</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="F33" s="15">
         <v>43660.868055555555</v>
@@ -4859,7 +4832,7 @@
       </c>
       <c r="E34" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>0.70138888888888884</v>
+        <v>0.84722222222222221</v>
       </c>
       <c r="F34" s="15">
         <v>43532.701388888891</v>
@@ -4884,7 +4857,7 @@
       </c>
       <c r="E35" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>0.90972222222222221</v>
+        <v>0.80555555555555547</v>
       </c>
       <c r="F35" s="15">
         <v>43719.652777777781</v>
@@ -4909,7 +4882,7 @@
       </c>
       <c r="E36" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>0.875</v>
+        <v>0.61111111111111105</v>
       </c>
       <c r="F36" s="15">
         <v>43756.583333333336</v>
@@ -4934,7 +4907,7 @@
       </c>
       <c r="E37" s="6">
         <f t="shared" ref="E37:E39" ca="1" si="10">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.70833333333333337</v>
+        <v>0.67361111111111116</v>
       </c>
       <c r="F37" s="15">
         <v>43542.888888888891</v>
@@ -4959,7 +4932,7 @@
       </c>
       <c r="E38" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>0.6875</v>
+        <v>0.90277777777777779</v>
       </c>
       <c r="F38" s="15">
         <v>43672.708333333336</v>
@@ -4984,7 +4957,7 @@
       </c>
       <c r="E39" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>0.71527777777777779</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="F39" s="15">
         <v>43423.902777777781</v>
@@ -5009,7 +4982,7 @@
       </c>
       <c r="E40" s="6">
         <f t="shared" ref="E40:E43" ca="1" si="11">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.90972222222222221</v>
+        <v>0.875</v>
       </c>
       <c r="F40" s="15">
         <v>43678.916666666664</v>
@@ -5034,7 +5007,7 @@
       </c>
       <c r="E41" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.65972222222222221</v>
+        <v>0.74305555555555547</v>
       </c>
       <c r="F41" s="15">
         <v>43514.958333333336</v>
@@ -5059,7 +5032,7 @@
       </c>
       <c r="E42" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.61111111111111105</v>
+        <v>0.88194444444444453</v>
       </c>
       <c r="F42" s="15">
         <v>43623.861111111109</v>
@@ -5084,7 +5057,7 @@
       </c>
       <c r="E43" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.6875</v>
+        <v>0.84027777777777779</v>
       </c>
       <c r="F43" s="15">
         <v>43701.722222222219</v>
@@ -5133,7 +5106,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C1" t="s">
         <v>239</v>
@@ -5148,14 +5121,14 @@
         <v>64</v>
       </c>
       <c r="G1" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="H1" t="e">
         <f>COUNT(#REF!)-COUNTIFS(#REF!,1)</f>
         <v>#REF!</v>
       </c>
       <c r="J1" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -6585,13 +6558,13 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <f ca="1">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.64583333333333337</v>
+        <v>0.81944444444444453</v>
       </c>
     </row>
   </sheetData>
@@ -6620,7 +6593,7 @@
         <v>200</v>
       </c>
       <c r="C1" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -12398,8 +12371,8 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -12445,14 +12418,14 @@
         <f>F2</f>
         <v>camilleconing@cinema.com</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="F2" s="1" t="str">
         <f>IF(G2=1,LOWER(D2&amp;E2)&amp;"@customers.com",LOWER(D2&amp;E2)&amp;"@cinema.com")</f>
@@ -12470,14 +12443,14 @@
         <f t="shared" ref="B3:B11" si="0">F3</f>
         <v>mattiealonso@cinema.com</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="F3" s="1" t="str">
         <f t="shared" ref="F3:F11" si="1">IF(G3=1,LOWER(D3&amp;E3)&amp;"@customers.com",LOWER(D3&amp;E3)&amp;"@cinema.com")</f>
@@ -12495,14 +12468,14 @@
         <f t="shared" si="0"/>
         <v>marylindigweed@cinema.com</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>253</v>
+      <c r="C4" s="10" t="s">
+        <v>279</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F4" s="1" t="str">
         <f t="shared" si="1"/>
@@ -12520,14 +12493,14 @@
         <f t="shared" si="0"/>
         <v>gerribeagles@cinema.com</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>256</v>
+      <c r="C5" s="10" t="s">
+        <v>279</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F5" s="1" t="str">
         <f t="shared" si="1"/>
@@ -12545,14 +12518,14 @@
         <f t="shared" si="0"/>
         <v>frannieyoskowitz@cinema.com</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>259</v>
+      <c r="C6" s="10" t="s">
+        <v>279</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="F6" s="1" t="str">
         <f t="shared" si="1"/>
@@ -12570,14 +12543,14 @@
         <f t="shared" si="0"/>
         <v>geoffscyone@customers.com</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>262</v>
+      <c r="C7" s="10" t="s">
+        <v>279</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="F7" s="1" t="str">
         <f t="shared" si="1"/>
@@ -12595,14 +12568,14 @@
         <f t="shared" si="0"/>
         <v>williebaxill@customers.com</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>265</v>
+      <c r="C8" s="10" t="s">
+        <v>279</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="F8" s="1" t="str">
         <f t="shared" si="1"/>
@@ -12620,14 +12593,14 @@
         <f t="shared" si="0"/>
         <v>laughtonskeldinge@customers.com</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>268</v>
+      <c r="C9" s="10" t="s">
+        <v>279</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="F9" s="1" t="str">
         <f t="shared" si="1"/>
@@ -12645,14 +12618,14 @@
         <f t="shared" si="0"/>
         <v>emiletheunissen@customers.com</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>271</v>
+      <c r="C10" s="10" t="s">
+        <v>279</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="F10" s="1" t="str">
         <f t="shared" si="1"/>
@@ -12670,14 +12643,14 @@
         <f t="shared" si="0"/>
         <v>jockbagwell@customers.com</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>274</v>
+      <c r="C11" s="10" t="s">
+        <v>279</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="F11" s="1" t="str">
         <f t="shared" si="1"/>
@@ -13234,7 +13207,7 @@
         <v>58</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -13383,7 +13356,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -13402,10 +13375,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="D1" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -13472,7 +13445,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>66</v>
@@ -13484,7 +13457,7 @@
         <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Fixed bug in TestBase SetUp
</commit_message>
<xml_diff>
--- a/Cinema.Test/TestDatabase/TestCinemaDatabase.xlsx
+++ b/Cinema.Test/TestDatabase/TestCinemaDatabase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Cinema\Cinema.Test\TestDatabase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Cinema - RS1\Cinema\Cinema.Test\TestDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754A2332-5722-4FB1-A8B0-2590CA07DF45}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AE7E14-DF33-4E4F-AC31-3047A2BAF114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="825" firstSheet="7" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pricings" sheetId="12" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="Users" sheetId="18" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Reservations!$B$1:$F$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Reservations'!$B$1:$F$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Seat!$A$1:$C$481</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">SeatReservations!$A$1:$E$62</definedName>
   </definedNames>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="279">
   <si>
     <t>Id</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>Administrator</t>
-  </si>
-  <si>
-    <t>Manager</t>
   </si>
   <si>
     <t>Title</t>
@@ -1292,7 +1289,7 @@
       <calculatedColumnFormula>INDEX(Screenings[Hall],MATCH(Reservations[[#This Row],[Test_Screening]],Screenings[Test_Id],0))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{02492577-30BC-4736-89A6-7BCB43316500}" name="Number of SeatReservations" dataDxfId="12" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>COUNTIF(SeatReservations!G:G,Reservations!G2)</calculatedColumnFormula>
+      <calculatedColumnFormula>COUNTIF(SeatReservations!G:G,'Reservations'!G2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{6629A0B4-1EED-4F00-8980-01C1615D1E46}" name="Movie" dataDxfId="11" dataCellStyle="Normal 2">
       <calculatedColumnFormula>INDEX(Screenings[Movie],MATCH(Reservations[[#This Row],[Test_Screening]],Screenings[Test_Id],0))</calculatedColumnFormula>
@@ -1614,8 +1611,8 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1632,7 +1629,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1640,7 +1637,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C2" s="3">
         <v>7</v>
@@ -1651,7 +1648,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="3">
         <v>8</v>
@@ -1662,7 +1659,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" s="3">
         <v>10</v>
@@ -1673,7 +1670,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="3">
         <v>6</v>
@@ -1684,7 +1681,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" s="3">
         <v>12</v>
@@ -1726,28 +1723,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1755,7 +1752,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" s="1">
         <v>108</v>
@@ -1764,16 +1761,16 @@
         <v>1995</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1781,7 +1778,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1">
         <v>127</v>
@@ -1790,16 +1787,16 @@
         <v>2012</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1807,7 +1804,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1">
         <v>158</v>
@@ -1816,16 +1813,16 @@
         <v>1970</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1833,7 +1830,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="1">
         <v>96</v>
@@ -1842,16 +1839,16 @@
         <v>1992</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1859,7 +1856,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="1">
         <v>119</v>
@@ -1868,16 +1865,16 @@
         <v>1970</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1885,7 +1882,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7" s="1">
         <v>160</v>
@@ -1894,16 +1891,16 @@
         <v>1971</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1911,7 +1908,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" s="1">
         <v>93</v>
@@ -1920,16 +1917,16 @@
         <v>1986</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1937,7 +1934,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" s="1">
         <v>68</v>
@@ -1946,16 +1943,16 @@
         <v>1980</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1963,7 +1960,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" s="1">
         <v>61</v>
@@ -1972,16 +1969,16 @@
         <v>2002</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1989,7 +1986,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C11" s="1">
         <v>96</v>
@@ -1998,16 +1995,16 @@
         <v>1992</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2015,7 +2012,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C12" s="1">
         <v>143</v>
@@ -2024,16 +2021,16 @@
         <v>2002</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2041,7 +2038,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="1">
         <v>115</v>
@@ -2050,16 +2047,16 @@
         <v>1968</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2096,19 +2093,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2116,13 +2113,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E2" s="1">
         <v>4</v>
@@ -2136,13 +2133,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" s="1">
         <v>4</v>
@@ -2156,13 +2153,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E4" s="1">
         <v>4</v>
@@ -2176,13 +2173,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
@@ -2196,13 +2193,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E6" s="1">
         <v>4</v>
@@ -2216,13 +2213,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E7" s="1">
         <v>4</v>
@@ -2236,13 +2233,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E8" s="1">
         <v>4</v>
@@ -2256,13 +2253,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E9" s="1">
         <v>4</v>
@@ -2276,13 +2273,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E10" s="1">
         <v>4</v>
@@ -2296,13 +2293,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E11" s="1">
         <v>4</v>
@@ -2345,16 +2342,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2362,7 +2359,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
@@ -2375,7 +2372,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -2385,7 +2382,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" s="1">
         <v>9</v>
@@ -2398,7 +2395,7 @@
         <v>4</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2406,7 +2403,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C4" s="1">
         <v>6</v>
@@ -2424,7 +2421,7 @@
         <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -2442,7 +2439,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C6" s="1">
         <v>10</v>
@@ -2460,7 +2457,7 @@
         <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
@@ -2478,7 +2475,7 @@
         <v>64</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C8" s="1">
         <v>9</v>
@@ -2496,7 +2493,7 @@
         <v>69</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -2514,7 +2511,7 @@
         <v>80</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C10" s="1">
         <v>8</v>
@@ -2532,7 +2529,7 @@
         <v>97</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -2550,7 +2547,7 @@
         <v>104</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C12" s="1">
         <v>10</v>
@@ -2568,7 +2565,7 @@
         <v>110</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -2586,7 +2583,7 @@
         <v>118</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C14" s="1">
         <v>9</v>
@@ -2604,7 +2601,7 @@
         <v>133</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C15" s="1">
         <v>3</v>
@@ -2622,7 +2619,7 @@
         <v>142</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C16" s="1">
         <v>6</v>
@@ -2640,7 +2637,7 @@
         <v>148</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C17" s="1">
         <v>6</v>
@@ -2658,7 +2655,7 @@
         <v>152</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
@@ -2676,7 +2673,7 @@
         <v>155</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C19" s="1">
         <v>4</v>
@@ -2694,7 +2691,7 @@
         <v>158</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C20" s="1">
         <v>9</v>
@@ -2712,7 +2709,7 @@
         <v>175</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C21" s="1">
         <v>10</v>
@@ -2730,7 +2727,7 @@
         <v>176</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C22" s="1">
         <v>7</v>
@@ -2748,7 +2745,7 @@
         <v>178</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -2766,7 +2763,7 @@
         <v>186</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C24" s="1">
         <v>10</v>
@@ -2784,7 +2781,7 @@
         <v>221</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C25" s="1">
         <v>8</v>
@@ -2802,7 +2799,7 @@
         <v>241</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C26" s="1">
         <v>9</v>
@@ -2820,7 +2817,7 @@
         <v>248</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C27" s="1">
         <v>3</v>
@@ -2838,7 +2835,7 @@
         <v>250</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
@@ -2856,7 +2853,7 @@
         <v>252</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C29" s="1">
         <v>10</v>
@@ -2874,7 +2871,7 @@
         <v>258</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C30" s="1">
         <v>4</v>
@@ -2892,7 +2889,7 @@
         <v>265</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C31" s="1">
         <v>5</v>
@@ -2910,7 +2907,7 @@
         <v>283</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C32" s="1">
         <v>4</v>
@@ -2928,7 +2925,7 @@
         <v>297</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
@@ -2946,7 +2943,7 @@
         <v>302</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C34" s="1">
         <v>10</v>
@@ -2964,7 +2961,7 @@
         <v>315</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C35" s="1">
         <v>6</v>
@@ -2982,7 +2979,7 @@
         <v>320</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C36" s="1">
         <v>4</v>
@@ -3000,7 +2997,7 @@
         <v>324</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C37" s="1">
         <v>5</v>
@@ -3018,7 +3015,7 @@
         <v>332</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C38" s="1">
         <v>3</v>
@@ -3036,7 +3033,7 @@
         <v>342</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C39" s="1">
         <v>5</v>
@@ -3054,7 +3051,7 @@
         <v>349</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C40" s="1">
         <v>5</v>
@@ -3101,28 +3098,28 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>276</v>
-      </c>
       <c r="D1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>155</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -3143,7 +3140,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G2)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G2)</f>
         <v>0</v>
       </c>
       <c r="F2" s="4">
@@ -3175,7 +3172,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G3)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G3)</f>
         <v>0</v>
       </c>
       <c r="F3" s="4">
@@ -3207,7 +3204,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G4)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G4)</f>
         <v>0</v>
       </c>
       <c r="F4" s="4">
@@ -3239,7 +3236,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G5)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G5)</f>
         <v>0</v>
       </c>
       <c r="F5" s="4">
@@ -3271,7 +3268,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G6)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G6)</f>
         <v>0</v>
       </c>
       <c r="F6" s="4">
@@ -3303,7 +3300,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G7)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G7)</f>
         <v>0</v>
       </c>
       <c r="F7" s="4">
@@ -3335,7 +3332,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G8)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G8)</f>
         <v>0</v>
       </c>
       <c r="F8" s="4">
@@ -3367,7 +3364,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G9)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G9)</f>
         <v>0</v>
       </c>
       <c r="F9" s="4">
@@ -3399,7 +3396,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G10)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G10)</f>
         <v>0</v>
       </c>
       <c r="F10" s="4">
@@ -3431,7 +3428,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G11)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G11)</f>
         <v>0</v>
       </c>
       <c r="F11" s="4">
@@ -3463,7 +3460,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G12)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G12)</f>
         <v>0</v>
       </c>
       <c r="F12" s="4">
@@ -3495,7 +3492,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G13)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G13)</f>
         <v>0</v>
       </c>
       <c r="F13" s="4">
@@ -3527,7 +3524,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G14)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G14)</f>
         <v>0</v>
       </c>
       <c r="F14" s="4">
@@ -3559,7 +3556,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G15)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G15)</f>
         <v>0</v>
       </c>
       <c r="F15" s="4">
@@ -3591,7 +3588,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G16)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G16)</f>
         <v>0</v>
       </c>
       <c r="F16" s="4">
@@ -3623,7 +3620,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G17)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G17)</f>
         <v>0</v>
       </c>
       <c r="F17" s="4">
@@ -3655,7 +3652,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G18)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G18)</f>
         <v>0</v>
       </c>
       <c r="F18" s="4">
@@ -3687,7 +3684,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G19)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G19)</f>
         <v>0</v>
       </c>
       <c r="F19" s="4">
@@ -3719,7 +3716,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G20)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G20)</f>
         <v>0</v>
       </c>
       <c r="F20" s="4">
@@ -3751,7 +3748,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G21)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G21)</f>
         <v>0</v>
       </c>
       <c r="F21" s="4">
@@ -3783,7 +3780,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G22)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G22)</f>
         <v>0</v>
       </c>
       <c r="F22" s="4">
@@ -3815,7 +3812,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G23)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G23)</f>
         <v>0</v>
       </c>
       <c r="F23" s="4">
@@ -3847,7 +3844,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G24)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G24)</f>
         <v>0</v>
       </c>
       <c r="F24" s="4">
@@ -3879,7 +3876,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G25)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G25)</f>
         <v>0</v>
       </c>
       <c r="F25" s="4">
@@ -3911,7 +3908,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G26)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G26)</f>
         <v>0</v>
       </c>
       <c r="F26" s="4">
@@ -3943,7 +3940,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="4">
-        <f>COUNTIF(SeatReservations!G:G,Reservations!G27)</f>
+        <f>COUNTIF(SeatReservations!G:G,'Reservations'!G27)</f>
         <v>0</v>
       </c>
       <c r="F27" s="4">
@@ -3995,22 +3992,22 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -4022,7 +4019,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -4032,7 +4029,7 @@
       </c>
       <c r="E2" s="6">
         <f t="shared" ref="E2" ca="1" si="0">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.85416666666666663</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="F2" s="15">
         <v>43513.618055555555</v>
@@ -4047,7 +4044,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -4057,7 +4054,7 @@
       </c>
       <c r="E3" s="6">
         <f t="shared" ref="E3:E6" ca="1" si="1">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.91666666666666663</v>
+        <v>0.57638888888888895</v>
       </c>
       <c r="F3" s="15">
         <v>43680.631944444445</v>
@@ -4072,7 +4069,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -4082,7 +4079,7 @@
       </c>
       <c r="E4" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85416666666666663</v>
+        <v>0.5625</v>
       </c>
       <c r="F4" s="15">
         <v>43698.944444444445</v>
@@ -4097,7 +4094,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -4107,7 +4104,7 @@
       </c>
       <c r="E5" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72916666666666663</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="F5" s="15">
         <v>43674.729166666664</v>
@@ -4122,7 +4119,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -4132,7 +4129,7 @@
       </c>
       <c r="E6" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80555555555555547</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="F6" s="15">
         <v>43730.590277777781</v>
@@ -4147,7 +4144,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -4157,7 +4154,7 @@
       </c>
       <c r="E7" s="6">
         <f t="shared" ref="E7:E8" ca="1" si="2">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.56944444444444442</v>
+        <v>0.57638888888888895</v>
       </c>
       <c r="F7" s="15">
         <v>43430.916666666664</v>
@@ -4172,7 +4169,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -4182,7 +4179,7 @@
       </c>
       <c r="E8" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>0.71527777777777779</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F8" s="15">
         <v>43674.826388888891</v>
@@ -4197,7 +4194,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -4207,7 +4204,7 @@
       </c>
       <c r="E9" s="6">
         <f t="shared" ref="E9" ca="1" si="3">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.875</v>
+        <v>0.59722222222222221</v>
       </c>
       <c r="F9" s="15">
         <v>43459.861111111109</v>
@@ -4222,7 +4219,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -4232,7 +4229,7 @@
       </c>
       <c r="E10" s="6">
         <f t="shared" ref="E10:E11" ca="1" si="4">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.66666666666666663</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="F10" s="15">
         <v>43531.555555555555</v>
@@ -4247,7 +4244,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -4257,7 +4254,7 @@
       </c>
       <c r="E11" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.61805555555555558</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="F11" s="15">
         <v>43552.6875</v>
@@ -4272,7 +4269,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -4282,7 +4279,7 @@
       </c>
       <c r="E12" s="6">
         <f t="shared" ref="E12:E18" ca="1" si="5">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.95138888888888884</v>
+        <v>0.86805555555555547</v>
       </c>
       <c r="F12" s="15">
         <v>43430.611111111109</v>
@@ -4297,7 +4294,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -4307,7 +4304,7 @@
       </c>
       <c r="E13" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.80555555555555547</v>
+        <v>0.71527777777777779</v>
       </c>
       <c r="F13" s="15">
         <v>43737.923611111109</v>
@@ -4322,7 +4319,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -4332,7 +4329,7 @@
       </c>
       <c r="E14" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.70138888888888884</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F14" s="15">
         <v>43705.868055555555</v>
@@ -4347,7 +4344,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -4357,7 +4354,7 @@
       </c>
       <c r="E15" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.94444444444444453</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="F15" s="15">
         <v>43738.881944444445</v>
@@ -4372,7 +4369,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -4382,7 +4379,7 @@
       </c>
       <c r="E16" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.56944444444444442</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F16" s="15">
         <v>43434.569444444445</v>
@@ -4397,7 +4394,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
@@ -4407,7 +4404,7 @@
       </c>
       <c r="E17" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.8125</v>
+        <v>0.94444444444444453</v>
       </c>
       <c r="F17" s="15">
         <v>43613.944444444445</v>
@@ -4422,7 +4419,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
@@ -4432,7 +4429,7 @@
       </c>
       <c r="E18" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.90972222222222221</v>
+        <v>0.93055555555555547</v>
       </c>
       <c r="F18" s="15">
         <v>43666.847222222219</v>
@@ -4447,7 +4444,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -4457,7 +4454,7 @@
       </c>
       <c r="E19" s="6">
         <f t="shared" ref="E19:E23" ca="1" si="6">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.95138888888888884</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="F19" s="15">
         <v>43694.951388888891</v>
@@ -4472,7 +4469,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
@@ -4482,7 +4479,7 @@
       </c>
       <c r="E20" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.8125</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F20" s="15">
         <v>43661.854166666664</v>
@@ -4497,7 +4494,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -4507,7 +4504,7 @@
       </c>
       <c r="E21" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.57638888888888895</v>
+        <v>0.8125</v>
       </c>
       <c r="F21" s="15">
         <v>43629.652777777781</v>
@@ -4522,7 +4519,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
@@ -4532,7 +4529,7 @@
       </c>
       <c r="E22" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.84722222222222221</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F22" s="15">
         <v>43430.847222222219</v>
@@ -4547,7 +4544,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -4557,7 +4554,7 @@
       </c>
       <c r="E23" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.64583333333333337</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="F23" s="15">
         <v>43632.618055555555</v>
@@ -4572,7 +4569,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
@@ -4582,7 +4579,7 @@
       </c>
       <c r="E24" s="6">
         <f t="shared" ref="E24:E29" ca="1" si="7">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.90972222222222221</v>
+        <v>0.89583333333333337</v>
       </c>
       <c r="F24" s="15">
         <v>43731.548611111109</v>
@@ -4597,7 +4594,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
@@ -4607,7 +4604,7 @@
       </c>
       <c r="E25" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.64583333333333337</v>
+        <v>0.68055555555555547</v>
       </c>
       <c r="F25" s="15">
         <v>43769.847222222219</v>
@@ -4622,7 +4619,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -4632,7 +4629,7 @@
       </c>
       <c r="E26" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.86111111111111116</v>
+        <v>0.90277777777777779</v>
       </c>
       <c r="F26" s="15">
         <v>43508.583333333336</v>
@@ -4647,7 +4644,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
@@ -4657,7 +4654,7 @@
       </c>
       <c r="E27" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.78472222222222221</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F27" s="15">
         <v>43441.548611111109</v>
@@ -4672,7 +4669,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
@@ -4682,7 +4679,7 @@
       </c>
       <c r="E28" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.84722222222222221</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="F28" s="15">
         <v>43725.75</v>
@@ -4697,7 +4694,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C29" s="1">
         <v>2</v>
@@ -4707,7 +4704,7 @@
       </c>
       <c r="E29" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.72222222222222221</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="F29" s="15">
         <v>43639.694444444445</v>
@@ -4722,7 +4719,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -4732,7 +4729,7 @@
       </c>
       <c r="E30" s="6">
         <f t="shared" ref="E30" ca="1" si="8">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.75</v>
+        <v>0.82638888888888884</v>
       </c>
       <c r="F30" s="15">
         <v>43704.902777777781</v>
@@ -4747,7 +4744,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C31" s="1">
         <v>2</v>
@@ -4757,7 +4754,7 @@
       </c>
       <c r="E31" s="6">
         <f t="shared" ref="E31:E36" ca="1" si="9">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.875</v>
+        <v>0.65972222222222221</v>
       </c>
       <c r="F31" s="15">
         <v>43727.638888888891</v>
@@ -4772,7 +4769,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
@@ -4782,7 +4779,7 @@
       </c>
       <c r="E32" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>0.64583333333333337</v>
+        <v>0.54861111111111105</v>
       </c>
       <c r="F32" s="15">
         <v>43773.715277777781</v>
@@ -4797,7 +4794,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -4807,7 +4804,7 @@
       </c>
       <c r="E33" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>0.65277777777777779</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F33" s="15">
         <v>43660.868055555555</v>
@@ -4822,7 +4819,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C34" s="1">
         <v>2</v>
@@ -4832,7 +4829,7 @@
       </c>
       <c r="E34" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>0.84722222222222221</v>
+        <v>0.8125</v>
       </c>
       <c r="F34" s="15">
         <v>43532.701388888891</v>
@@ -4847,7 +4844,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
@@ -4857,7 +4854,7 @@
       </c>
       <c r="E35" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>0.80555555555555547</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="F35" s="15">
         <v>43719.652777777781</v>
@@ -4872,7 +4869,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C36" s="1">
         <v>2</v>
@@ -4882,7 +4879,7 @@
       </c>
       <c r="E36" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>0.61111111111111105</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F36" s="15">
         <v>43756.583333333336</v>
@@ -4897,7 +4894,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C37" s="1">
         <v>2</v>
@@ -4907,7 +4904,7 @@
       </c>
       <c r="E37" s="6">
         <f t="shared" ref="E37:E39" ca="1" si="10">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.67361111111111116</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="F37" s="15">
         <v>43542.888888888891</v>
@@ -4922,7 +4919,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
@@ -4932,7 +4929,7 @@
       </c>
       <c r="E38" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>0.90277777777777779</v>
+        <v>0.70138888888888884</v>
       </c>
       <c r="F38" s="15">
         <v>43672.708333333336</v>
@@ -4947,7 +4944,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C39" s="1">
         <v>2</v>
@@ -4957,7 +4954,7 @@
       </c>
       <c r="E39" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>0.85416666666666663</v>
+        <v>0.84027777777777779</v>
       </c>
       <c r="F39" s="15">
         <v>43423.902777777781</v>
@@ -4972,7 +4969,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C40" s="1">
         <v>2</v>
@@ -4982,7 +4979,7 @@
       </c>
       <c r="E40" s="6">
         <f t="shared" ref="E40:E43" ca="1" si="11">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.875</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="F40" s="15">
         <v>43678.916666666664</v>
@@ -4997,7 +4994,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
@@ -5007,7 +5004,7 @@
       </c>
       <c r="E41" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.74305555555555547</v>
+        <v>0.8125</v>
       </c>
       <c r="F41" s="15">
         <v>43514.958333333336</v>
@@ -5022,7 +5019,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C42" s="1">
         <v>2</v>
@@ -5032,7 +5029,7 @@
       </c>
       <c r="E42" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.88194444444444453</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="F42" s="15">
         <v>43623.861111111109</v>
@@ -5047,7 +5044,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
@@ -5057,7 +5054,7 @@
       </c>
       <c r="E43" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.84027777777777779</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="F43" s="15">
         <v>43701.722222222219</v>
@@ -5106,29 +5103,29 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>240</v>
-      </c>
       <c r="F1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H1" t="e">
         <f>COUNT(#REF!)-COUNTIFS(#REF!,1)</f>
         <v>#REF!</v>
       </c>
       <c r="J1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -6558,13 +6555,13 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <f ca="1">TIME(RANDBETWEEN(13,22),ROUNDUP(RANDBETWEEN(0,59),-1),0)</f>
-        <v>0.81944444444444453</v>
+        <v>0.55555555555555558</v>
       </c>
     </row>
   </sheetData>
@@ -6590,10 +6587,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -12371,8 +12368,8 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -12392,22 +12389,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -12419,20 +12416,20 @@
         <v>camilleconing@cinema.com</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="F2" s="1" t="str">
         <f>IF(G2=1,LOWER(D2&amp;E2)&amp;"@customers.com",LOWER(D2&amp;E2)&amp;"@cinema.com")</f>
         <v>camilleconing@cinema.com</v>
       </c>
       <c r="G2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -12441,23 +12438,23 @@
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" ref="B3:B11" si="0">F3</f>
-        <v>mattiealonso@cinema.com</v>
+        <v>mattiealonso@customers.com</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="F3" s="1" t="str">
         <f t="shared" ref="F3:F11" si="1">IF(G3=1,LOWER(D3&amp;E3)&amp;"@customers.com",LOWER(D3&amp;E3)&amp;"@cinema.com")</f>
-        <v>mattiealonso@cinema.com</v>
+        <v>mattiealonso@customers.com</v>
       </c>
       <c r="G3" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -12466,23 +12463,23 @@
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>marylindigweed@cinema.com</v>
+        <v>marylindigweed@customers.com</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="F4" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>marylindigweed@cinema.com</v>
+        <v>marylindigweed@customers.com</v>
       </c>
       <c r="G4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -12494,13 +12491,13 @@
         <v>gerribeagles@cinema.com</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="F5" s="1" t="str">
         <f t="shared" si="1"/>
@@ -12519,13 +12516,13 @@
         <v>frannieyoskowitz@cinema.com</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="F6" s="1" t="str">
         <f t="shared" si="1"/>
@@ -12544,13 +12541,13 @@
         <v>geoffscyone@customers.com</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>258</v>
       </c>
       <c r="F7" s="1" t="str">
         <f t="shared" si="1"/>
@@ -12569,13 +12566,13 @@
         <v>williebaxill@customers.com</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="F8" s="1" t="str">
         <f t="shared" si="1"/>
@@ -12594,13 +12591,13 @@
         <v>laughtonskeldinge@customers.com</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="F9" s="1" t="str">
         <f t="shared" si="1"/>
@@ -12619,13 +12616,13 @@
         <v>emiletheunissen@customers.com</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="F10" s="1" t="str">
         <f t="shared" si="1"/>
@@ -12644,13 +12641,13 @@
         <v>jockbagwell@customers.com</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="F11" s="1" t="str">
         <f t="shared" si="1"/>
@@ -12694,7 +12691,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -12702,7 +12699,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -12710,7 +12707,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -12718,7 +12715,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -12726,7 +12723,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -12739,10 +12736,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12777,14 +12774,6 @@
       </c>
       <c r="B4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -12821,25 +12810,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -12847,13 +12836,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E2" s="1">
         <v>4</v>
@@ -12862,7 +12851,7 @@
         <v>43749</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
@@ -12873,13 +12862,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E3" s="1">
         <v>4</v>
@@ -12888,7 +12877,7 @@
         <v>43581</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1">
         <v>3</v>
@@ -12900,13 +12889,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E4" s="1">
         <v>4</v>
@@ -12915,7 +12904,7 @@
         <v>43708</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="1">
         <v>2</v>
@@ -12927,13 +12916,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
@@ -12942,7 +12931,7 @@
         <v>43590</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="1">
         <v>4</v>
@@ -12954,13 +12943,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E6" s="1">
         <v>4</v>
@@ -12969,7 +12958,7 @@
         <v>43723</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="1">
         <v>2</v>
@@ -12981,13 +12970,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="E7" s="1">
         <v>4</v>
@@ -12996,7 +12985,7 @@
         <v>43675</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="1">
         <v>2</v>
@@ -13008,13 +12997,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="E8" s="1">
         <v>4</v>
@@ -13023,7 +13012,7 @@
         <v>43690</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="1">
         <v>4</v>
@@ -13035,13 +13024,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E9" s="1">
         <v>4</v>
@@ -13050,7 +13039,7 @@
         <v>43582</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H9" s="1">
         <v>4</v>
@@ -13062,13 +13051,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="E10" s="1">
         <v>4</v>
@@ -13077,7 +13066,7 @@
         <v>43634</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H10" s="1">
         <v>4</v>
@@ -13089,13 +13078,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="E11" s="1">
         <v>4</v>
@@ -13104,7 +13093,7 @@
         <v>43550</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" s="1">
         <v>1</v>
@@ -13145,7 +13134,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -13153,7 +13142,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -13161,7 +13150,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -13169,7 +13158,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -13201,13 +13190,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="D1" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -13322,7 +13311,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -13330,7 +13319,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -13338,7 +13327,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -13375,10 +13364,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" t="s">
         <v>273</v>
-      </c>
-      <c r="D1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -13386,7 +13375,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2">
         <v>16</v>
@@ -13400,7 +13389,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3">
         <v>16</v>
@@ -13445,22 +13434,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I1" s="1"/>
     </row>

</xml_diff>